<commit_message>
verification update - path issue fixed
</commit_message>
<xml_diff>
--- a/notebooks/mkappa/verification_data/Rem20/Abbildung_4-9/Rempel_2018_4-9.xlsx
+++ b/notebooks/mkappa/verification_data/Rem20/Abbildung_4-9/Rempel_2018_4-9.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srate\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IMB\PyCharm_workspace\bmcs_cross_section\notebooks\mkappa\verification_data\Rem20\Abbildung_4-9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB62EEA5-FB1C-4C77-B7D1-DBFABEA7100D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B7590D-12D0-4F51-9C77-BD3D083C383D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="10800" windowHeight="8780" xr2:uid="{F14F4C78-6418-471D-B0D9-8A16E22AACAF}"/>
+    <workbookView xWindow="6520" yWindow="1020" windowWidth="10800" windowHeight="8780" xr2:uid="{F14F4C78-6418-471D-B0D9-8A16E22AACAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,6 +49,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -78,13 +81,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -401,15 +407,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7299FF-96B6-464A-BDE4-D88D26FEF539}">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -425,7 +435,7 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -447,7 +457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3.1578947368421053E-4</v>
       </c>
@@ -469,7 +479,7 @@
         <v>1.4274509803921569</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>1.2631578947368421E-3</v>
       </c>
@@ -491,7 +501,7 @@
         <v>2.1686274509803924</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>1.8947368421052631E-3</v>
       </c>
@@ -513,7 +523,7 @@
         <v>2.003921568627451</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>3.1578947368421048E-3</v>
       </c>
@@ -535,7 +545,7 @@
         <v>2.9098039215686278</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>4.4210526315789471E-3</v>
       </c>
@@ -556,8 +566,14 @@
       <c r="H8" s="3">
         <v>2.7450980392156863</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>5.3684210526315787E-3</v>
       </c>
@@ -578,8 +594,14 @@
       <c r="H9" s="3">
         <v>2.6901960784313728</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J9" s="4">
+        <v>0.26168224299065418</v>
+      </c>
+      <c r="K9" s="4">
+        <v>10.3125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>6.9473684210526309E-3</v>
       </c>
@@ -600,8 +622,14 @@
       <c r="H10" s="3">
         <v>2.9647058823529413</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J10" s="4">
+        <v>3.3457943925233646</v>
+      </c>
+      <c r="K10" s="4">
+        <v>14.625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>7.5789473684210523E-3</v>
       </c>
@@ -622,8 +650,14 @@
       <c r="H11" s="3">
         <v>3.1568627450980391</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J11" s="4">
+        <v>0.22429906542056074</v>
+      </c>
+      <c r="K11" s="4">
+        <v>4.8125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>8.8421052631578942E-3</v>
       </c>
@@ -645,7 +679,7 @@
         <v>3.4039215686274509</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>9.4736842105263147E-3</v>
       </c>
@@ -667,7 +701,7 @@
         <v>3.0470588235294116</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>1.0736842105263157E-2</v>
       </c>
@@ -689,7 +723,7 @@
         <v>3.4588235294117649</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>1.2E-2</v>
       </c>
@@ -711,7 +745,7 @@
         <v>3.2941176470588234</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>1.2947368421052631E-2</v>
       </c>
@@ -1567,5 +1601,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>